<commit_message>
Updates to curve fitting functions...
</commit_message>
<xml_diff>
--- a/GlobalReserves/BalSheets/ECBASSETSW.xlsx
+++ b/GlobalReserves/BalSheets/ECBASSETSW.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1346"/>
+  <dimension ref="A1:G1350"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34080,7 +34080,11 @@
       <c r="A1346" s="2" t="n">
         <v>45282</v>
       </c>
-      <c r="B1346" t="inlineStr"/>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>:ECBASSETSW</t>
+        </is>
+      </c>
       <c r="C1346" t="n">
         <v>6899165000000</v>
       </c>
@@ -34094,6 +34098,90 @@
         <v>6899165000000</v>
       </c>
       <c r="G1346" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" s="2" t="n">
+        <v>45282</v>
+      </c>
+      <c r="B1347" t="inlineStr"/>
+      <c r="C1347" t="n">
+        <v>6899165000000</v>
+      </c>
+      <c r="D1347" t="n">
+        <v>6899165000000</v>
+      </c>
+      <c r="E1347" t="n">
+        <v>6899165000000</v>
+      </c>
+      <c r="F1347" t="n">
+        <v>6899165000000</v>
+      </c>
+      <c r="G1347" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" s="2" t="n">
+        <v>45289</v>
+      </c>
+      <c r="B1348" t="inlineStr"/>
+      <c r="C1348" t="n">
+        <v>6935489000000</v>
+      </c>
+      <c r="D1348" t="n">
+        <v>6935489000000</v>
+      </c>
+      <c r="E1348" t="n">
+        <v>6935489000000</v>
+      </c>
+      <c r="F1348" t="n">
+        <v>6935489000000</v>
+      </c>
+      <c r="G1348" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" s="2" t="n">
+        <v>45296</v>
+      </c>
+      <c r="B1349" t="inlineStr"/>
+      <c r="C1349" t="n">
+        <v>6919847000000</v>
+      </c>
+      <c r="D1349" t="n">
+        <v>6919847000000</v>
+      </c>
+      <c r="E1349" t="n">
+        <v>6919847000000</v>
+      </c>
+      <c r="F1349" t="n">
+        <v>6919847000000</v>
+      </c>
+      <c r="G1349" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" s="2" t="n">
+        <v>45303</v>
+      </c>
+      <c r="B1350" t="inlineStr"/>
+      <c r="C1350" t="n">
+        <v>6923651000000</v>
+      </c>
+      <c r="D1350" t="n">
+        <v>6923651000000</v>
+      </c>
+      <c r="E1350" t="n">
+        <v>6923651000000</v>
+      </c>
+      <c r="F1350" t="n">
+        <v>6923651000000</v>
+      </c>
+      <c r="G1350" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>